<commit_message>
agregando estilos a la tabla de validaciones
</commit_message>
<xml_diff>
--- a/reportes/file03.xlsx
+++ b/reportes/file03.xlsx
@@ -414,7 +414,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="str">
-        <f>B2/(12*453)</f>
+        <f>B2/(12*1000)</f>
         <v>0</v>
       </c>
     </row>
@@ -423,7 +423,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="str">
-        <f>B3/(12*453)</f>
+        <f>B3/(12*1000)</f>
         <v>0</v>
       </c>
     </row>
@@ -432,7 +432,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.081795086880531</v>
+        <v>0.080189449009009</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -440,7 +440,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>31.410433703456</v>
+        <v>43.773064159559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregando detalles de mejora
</commit_message>
<xml_diff>
--- a/reportes/file03.xlsx
+++ b/reportes/file03.xlsx
@@ -398,7 +398,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>NAN</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -406,25 +406,25 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>69.067664339705</v>
+        <v>NAN</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <f>B2/(12*95)</f>
-        <v>0.087719298245614</v>
+      <c r="B4" t="str">
+        <f>B2/(12*6548)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <f>B3/(12*95)</f>
-        <v>0.060585670473425</v>
+      <c r="B5" t="str">
+        <f>B3/(12*6548)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -432,7 +432,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.082048508723404</v>
+        <v>0.08300413274935</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -440,7 +440,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>15.507313055867</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>